<commit_message>
File update after write data into it.
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>FirstName</t>
   </si>
@@ -76,12 +76,19 @@
   </si>
   <si>
     <t>SDET</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Jackson</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -447,7 +454,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -456,58 +463,73 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>5</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>200000.0</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>8</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>110000.0</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>11</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>135000.0</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>14</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>125000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>